<commit_message>
ENTREGA DO QUARTO SPRINT
</commit_message>
<xml_diff>
--- a/documentacao/BurnDown/04_burndownQuartoSprint.xlsx
+++ b/documentacao/BurnDown/04_burndownQuartoSprint.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\TCC\documentacao\BurnDown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F0B5D1-D112-49DA-A5F1-EA855C804500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A792075-2362-41C8-9687-BE98DDF99478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,7 +242,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -265,11 +265,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -278,6 +358,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -985,7 +1074,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="95000"/>
@@ -1005,13 +1094,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="pt-BR"/>
-              <a:t>Burn</a:t>
+              <a:t>Burn Down Chart</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="pt-BR" baseline="0"/>
-              <a:t> Down Chart</a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1028,7 +1112,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+            <a:defRPr sz="1680" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="95000"/>
@@ -1341,7 +1425,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="85000"/>
@@ -1399,7 +1483,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="85000"/>
@@ -1440,7 +1524,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="85000"/>
@@ -1497,7 +1581,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1400" baseline="0"/>
       </a:pPr>
       <a:endParaRPr lang="pt-BR"/>
     </a:p>
@@ -2970,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3958,37 +4042,37 @@
       <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>6</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="7">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7">
         <v>2</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
+      <c r="E18" s="7">
+        <v>0</v>
+      </c>
+      <c r="F18" s="7">
         <v>2</v>
       </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
+      <c r="G18" s="7">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1</v>
+      </c>
+      <c r="I18" s="7">
+        <v>0</v>
+      </c>
+      <c r="J18" s="7">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="12">
         <v>0</v>
       </c>
     </row>
@@ -3996,37 +4080,37 @@
       <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="8">
         <v>5</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
+      <c r="C19" s="9">
+        <v>0</v>
+      </c>
+      <c r="D19" s="9">
+        <v>1</v>
+      </c>
+      <c r="E19" s="9">
         <v>2</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>1</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
+      <c r="F19" s="9">
+        <v>0</v>
+      </c>
+      <c r="G19" s="9">
+        <v>1</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0</v>
+      </c>
+      <c r="J19" s="9">
+        <v>1</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="13">
         <v>0</v>
       </c>
     </row>
@@ -4034,37 +4118,37 @@
       <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="8">
         <v>5</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
+      <c r="C20" s="9">
+        <v>0</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0</v>
+      </c>
+      <c r="I20" s="9">
         <v>2</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="9">
         <v>3</v>
       </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
+      <c r="K20" s="9">
+        <v>0</v>
+      </c>
+      <c r="L20" s="13">
         <v>0</v>
       </c>
     </row>
@@ -4072,37 +4156,37 @@
       <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="8">
         <v>6</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
+      <c r="C21" s="9">
+        <v>0</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0</v>
+      </c>
+      <c r="G21" s="9">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0</v>
+      </c>
+      <c r="I21" s="9">
         <v>2</v>
       </c>
-      <c r="J21">
-        <v>0</v>
-      </c>
-      <c r="K21">
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
+      <c r="K21" s="9">
         <v>3</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4110,37 +4194,37 @@
       <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="8">
         <v>3</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
         <v>2</v>
       </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
+      <c r="D22" s="9">
+        <v>0</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0</v>
+      </c>
+      <c r="I22" s="9">
+        <v>0</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0</v>
+      </c>
+      <c r="L22" s="13">
         <v>0</v>
       </c>
     </row>
@@ -4148,37 +4232,37 @@
       <c r="A23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="8">
         <v>3</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
+      <c r="C23" s="9">
+        <v>0</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0</v>
+      </c>
+      <c r="E23" s="9">
         <v>2</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
+      <c r="F23" s="9">
+        <v>1</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0</v>
+      </c>
+      <c r="I23" s="9">
+        <v>0</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0</v>
+      </c>
+      <c r="L23" s="13">
         <v>0</v>
       </c>
     </row>
@@ -4186,37 +4270,37 @@
       <c r="A24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="8">
         <v>6</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
+      <c r="C24" s="9">
+        <v>0</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0</v>
+      </c>
+      <c r="E24" s="9">
+        <v>0</v>
+      </c>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9">
         <v>2</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
+      <c r="I24" s="9">
+        <v>1</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0</v>
+      </c>
+      <c r="K24" s="9">
         <v>2</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="13">
         <v>0</v>
       </c>
     </row>
@@ -4224,37 +4308,37 @@
       <c r="A25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="8">
         <v>6</v>
       </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>0</v>
-      </c>
-      <c r="I25">
+      <c r="C25" s="9">
+        <v>0</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0</v>
+      </c>
+      <c r="E25" s="9">
+        <v>0</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0</v>
+      </c>
+      <c r="I25" s="9">
         <v>2</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="9">
         <v>2</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="9">
         <v>2</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="13">
         <v>0</v>
       </c>
     </row>
@@ -4262,37 +4346,37 @@
       <c r="A26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="8">
         <v>5</v>
       </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26">
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
         <v>2</v>
       </c>
-      <c r="H26">
-        <v>0</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
         <v>2</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4300,37 +4384,37 @@
       <c r="A27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="8">
         <v>10</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-      <c r="K27">
-        <v>1</v>
-      </c>
-      <c r="L27">
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9">
+        <v>1</v>
+      </c>
+      <c r="H27" s="9">
+        <v>1</v>
+      </c>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
+      <c r="J27" s="9">
+        <v>1</v>
+      </c>
+      <c r="K27" s="9">
+        <v>1</v>
+      </c>
+      <c r="L27" s="13">
         <v>1</v>
       </c>
     </row>
@@ -4338,47 +4422,47 @@
       <c r="A28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="8">
         <f>SUM(B18:B27)</f>
         <v>55</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="9">
         <f>IF(SUM(C18:C27)&gt;0,B28-SUM(C18:C27),"")</f>
         <v>51</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="9">
         <f>IF(SUM(D18:D27)&gt;0,C28-SUM(D18:D27),"")</f>
         <v>47</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="9">
         <f>IF(SUM(E18:E27)&gt;0,D28-SUM(E18:E27),"")</f>
         <v>41</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="9">
         <f>IF(SUM(F18:F27)&gt;0,E28-SUM(F18:F27),"")</f>
         <v>36</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="9">
         <f>IF(SUM(G18:G27)&gt;0,F28-SUM(G18:G27),"")</f>
         <v>32</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="9">
         <f t="shared" ref="H28:L28" si="9">IF(SUM(H18:H27)&gt;0,G28-SUM(H18:H27),"")</f>
         <v>28</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="9">
         <f t="shared" si="9"/>
         <v>20</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="9">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="9">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="13">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
@@ -4387,47 +4471,47 @@
       <c r="A29" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="10">
         <f>B28</f>
         <v>55</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="11">
         <f>B29-($B$29/COUNTA($C$17:$L$17))</f>
         <v>49.5</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="11">
         <f t="shared" ref="D29:L29" si="10">C29-($B$29/COUNTA($C$17:$L$17))</f>
         <v>44</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="11">
         <f t="shared" si="10"/>
         <v>38.5</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="11">
         <f t="shared" si="10"/>
         <v>33</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="11">
         <f t="shared" si="10"/>
         <v>27.5</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="11">
         <f t="shared" si="10"/>
         <v>22</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="11">
         <f t="shared" si="10"/>
         <v>16.5</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="11">
         <f t="shared" si="10"/>
         <v>11</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="11">
         <f t="shared" si="10"/>
         <v>5.5</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="14">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>

</xml_diff>